<commit_message>
adding apis related hqm_quiz
</commit_message>
<xml_diff>
--- a/Data_Config/API_Data.xlsx
+++ b/Data_Config/API_Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdi/OneDrive - Deloitte (O365D)/Training/Main_API_Project/Data_Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BEF49D-F00E-1943-B707-8D54D90A2942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E595297D-67A7-9D48-B626-9FD6E3D6042E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" activeTab="1" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="Admin_Quiz" sheetId="3" r:id="rId2"/>
+    <sheet name="User" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
   <si>
     <t>password</t>
   </si>
@@ -290,6 +292,72 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>add_single_quiz</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>categoryId</t>
+  </si>
+  <si>
+    <t>add_category</t>
+  </si>
+  <si>
+    <t>Java Core</t>
+  </si>
+  <si>
+    <t>get_all_questions</t>
+  </si>
+  <si>
+    <t>question_number</t>
+  </si>
+  <si>
+    <t>update_a_question</t>
+  </si>
+  <si>
+    <t>delete_a_question</t>
+  </si>
+  <si>
+    <t>add_question</t>
+  </si>
+  <si>
+    <t>save_hux</t>
+  </si>
+  <si>
+    <t>huBatchTitle</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>=RANDBETWEEN(10,100)</t>
+  </si>
+  <si>
+    <t>2022-01-10</t>
+  </si>
+  <si>
+    <t>2022-02-14</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>get_all_hux</t>
+  </si>
+  <si>
+    <t>get_alluser_by_huid</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>1234@admin</t>
   </si>
 </sst>
 </file>
@@ -340,13 +408,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -991,10 +1060,202 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6600EE46-6C5A-6649-A34E-9FDADEE27C97}">
+  <dimension ref="A1:T11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="12" max="12" width="65.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{677BBBB2-6390-CD4A-A982-BC5BB612C02A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7C33C-1E6F-EF46-87FC-597C7CD0D47D}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1027,8 +1288,12 @@
       <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1079,6 +1344,9 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1087,7 +1355,9 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>

</xml_diff>

<commit_message>
Changes done in Login file
</commit_message>
<xml_diff>
--- a/Data_Config/API_Data.xlsx
+++ b/Data_Config/API_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdi/OneDrive - Deloitte (O365D)/Training/Main_API_Project/Data_Config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohdsalekhan/Documents/HQM_API/Main_Project_API/Data_Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F53C86-1CCA-E742-9F5F-7ECC876815CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7F1D6-93E3-C24C-8873-D7F6240A3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" activeTab="1" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="5" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="185">
   <si>
     <t>password</t>
   </si>
@@ -454,6 +454,147 @@
   </si>
   <si>
     <t>application/json</t>
+  </si>
+  <si>
+    <t>Register_user_kakashi</t>
+  </si>
+  <si>
+    <t>Kakashi</t>
+  </si>
+  <si>
+    <t>Hatake</t>
+  </si>
+  <si>
+    <t>kakashi@gmail.com</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>passwordfghj</t>
+  </si>
+  <si>
+    <t>Register_user_itachi</t>
+  </si>
+  <si>
+    <t>Itachi</t>
+  </si>
+  <si>
+    <t>Uchiha</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>itachi@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_itachi123</t>
+  </si>
+  <si>
+    <t>Itachi123</t>
+  </si>
+  <si>
+    <t>Itachiiii</t>
+  </si>
+  <si>
+    <t>Uchihaaa</t>
+  </si>
+  <si>
+    <t>itachi123@gmail.com</t>
+  </si>
+  <si>
+    <t>0987652321</t>
+  </si>
+  <si>
+    <t>Register_user_naruto</t>
+  </si>
+  <si>
+    <t>naruto</t>
+  </si>
+  <si>
+    <t>uzumaki</t>
+  </si>
+  <si>
+    <t>098765431</t>
+  </si>
+  <si>
+    <t>naruto@gmail.com</t>
+  </si>
+  <si>
+    <t>0987652311</t>
+  </si>
+  <si>
+    <t>Register_user_madara</t>
+  </si>
+  <si>
+    <t>madara</t>
+  </si>
+  <si>
+    <t>madara@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_hashirama</t>
+  </si>
+  <si>
+    <t>hashirama</t>
+  </si>
+  <si>
+    <t>senju</t>
+  </si>
+  <si>
+    <t>hashirama@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_hinata</t>
+  </si>
+  <si>
+    <t>hinata</t>
+  </si>
+  <si>
+    <t>hyuga</t>
+  </si>
+  <si>
+    <t>hinata@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_gara</t>
+  </si>
+  <si>
+    <t>gara</t>
+  </si>
+  <si>
+    <t>gara@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_asuma</t>
+  </si>
+  <si>
+    <t>asuma</t>
+  </si>
+  <si>
+    <t>sarutobi</t>
+  </si>
+  <si>
+    <t>asuma@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_yamato</t>
+  </si>
+  <si>
+    <t>yamato</t>
+  </si>
+  <si>
+    <t>yamato@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_user_sakura</t>
+  </si>
+  <si>
+    <t>sakura</t>
+  </si>
+  <si>
+    <t>sakura@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7E34A6-71B8-1D4A-A950-D36CAC193DC9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1277,7 +1418,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1577,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7C33C-1E6F-EF46-87FC-597C7CD0D47D}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1696,14 +1837,33 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1717,14 +1877,33 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1738,14 +1917,33 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1758,9 +1956,252 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{DD9AC12A-7417-8743-AB1C-FB29DF59CC2E}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{A3AAA2CF-F2DD-AA4E-8A57-609CAE06519F}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{94486D53-3009-CD44-82A0-AB234BD63390}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{D6AF9886-14F4-C542-88AA-534AA98EB39D}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{3D300B63-FB45-8441-91C5-3365DC98163D}"/>
+    <hyperlink ref="F8" r:id="rId6" display="itachi123@gmail.com" xr:uid="{27EE8E52-795C-3D40-8528-DE284B27AB98}"/>
+    <hyperlink ref="F9" r:id="rId7" display="mailto:itachi123@gmail.com" xr:uid="{2E190F26-51D8-4448-8A70-D9F22325C948}"/>
+    <hyperlink ref="F10" r:id="rId8" display="mailto:itachi123@gmail.com" xr:uid="{02613AA4-612D-124C-8ECE-AAB4E3B8EC84}"/>
+    <hyperlink ref="F11" r:id="rId9" display="mailto:itachi123@gmail.com" xr:uid="{40C03F1A-7811-7A40-8959-3EBD3B8C2F0D}"/>
+    <hyperlink ref="F12" r:id="rId10" display="mailto:itachi123@gmail.com" xr:uid="{AB5771FA-B405-3D43-AD83-5031AEA235EB}"/>
+    <hyperlink ref="F13" r:id="rId11" display="mailto:itachi123@gmail.com" xr:uid="{45C0D301-2445-8F41-A663-9E22C2937DAD}"/>
+    <hyperlink ref="F14" r:id="rId12" display="mailto:itachi123@gmail.com" xr:uid="{7742987C-FA32-4D40-8DE2-0E0B85A57152}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the code with comment changes
</commit_message>
<xml_diff>
--- a/Data_Config/API_Data.xlsx
+++ b/Data_Config/API_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohdsalekhan/Documents/HQM_API/Main_Project_API/Data_Config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/submg/Desktop/untitled folder/Main_Project_API/Data_Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7F1D6-93E3-C24C-8873-D7F6240A3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8973683D-4D7F-FA4C-AA94-B9230CAB65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="5" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="3" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="194">
   <si>
     <t>password</t>
   </si>
@@ -595,6 +595,33 @@
   </si>
   <si>
     <t>sakura@gmail.com</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>0987652333</t>
+  </si>
+  <si>
+    <t>Register_user_black</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>black@gmail.com</t>
+  </si>
+  <si>
+    <t>0987652330</t>
+  </si>
+  <si>
+    <t>Register_user_white</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>white@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1499,11 +1526,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0445D9-8284-D64B-BDC6-D6BF53F5BB89}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
@@ -1718,19 +1749,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7C33C-1E6F-EF46-87FC-597C7CD0D47D}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -1756,12 +1788,14 @@
         <v>78</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1771,8 +1805,9 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1809,8 +1844,9 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -1822,10 +1858,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1835,8 +1871,9 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="2" t="s">
         <v>138</v>
       </c>
@@ -1864,7 +1901,6 @@
       <c r="I4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1875,8 +1911,9 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>144</v>
       </c>
@@ -1904,7 +1941,6 @@
       <c r="I5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1915,8 +1951,9 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>149</v>
       </c>
@@ -1944,7 +1981,6 @@
       <c r="I6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1955,8 +1991,9 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>155</v>
       </c>
@@ -1985,7 +2022,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>161</v>
       </c>
@@ -2014,7 +2051,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="5" t="s">
         <v>164</v>
       </c>
@@ -2043,7 +2080,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>168</v>
       </c>
@@ -2072,7 +2109,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="5" t="s">
         <v>172</v>
       </c>
@@ -2101,7 +2138,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>175</v>
       </c>
@@ -2130,7 +2167,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>179</v>
       </c>
@@ -2159,7 +2196,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>182</v>
       </c>
@@ -2179,12 +2216,70 @@
         <v>184</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>84</v>
       </c>
       <c r="I14" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2202,6 +2297,8 @@
     <hyperlink ref="F12" r:id="rId10" display="mailto:itachi123@gmail.com" xr:uid="{AB5771FA-B405-3D43-AD83-5031AEA235EB}"/>
     <hyperlink ref="F13" r:id="rId11" display="mailto:itachi123@gmail.com" xr:uid="{45C0D301-2445-8F41-A663-9E22C2937DAD}"/>
     <hyperlink ref="F14" r:id="rId12" display="mailto:itachi123@gmail.com" xr:uid="{7742987C-FA32-4D40-8DE2-0E0B85A57152}"/>
+    <hyperlink ref="F15" r:id="rId13" display="mailto:itachi123@gmail.com" xr:uid="{68383A25-34AD-4447-926A-730E5EA471C2}"/>
+    <hyperlink ref="F16" r:id="rId14" display="mailto:itachi123@gmail.com" xr:uid="{965C944F-B357-9C4C-9640-B3128A846A21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the registration code
</commit_message>
<xml_diff>
--- a/Data_Config/API_Data.xlsx
+++ b/Data_Config/API_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohdsalekhan/Documents/HQM_API/Main_Project_API/Data_Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7F1D6-93E3-C24C-8873-D7F6240A3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0973C381-9F9E-FF4D-8678-A621A373C06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="5" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="191">
   <si>
     <t>password</t>
   </si>
@@ -595,6 +595,24 @@
   </si>
   <si>
     <t>sakura@gmail.com</t>
+  </si>
+  <si>
+    <t>Register_usernew</t>
+  </si>
+  <si>
+    <t>Saleem Mo</t>
+  </si>
+  <si>
+    <t>saleemnew</t>
+  </si>
+  <si>
+    <t>khannew</t>
+  </si>
+  <si>
+    <t>testnew@test.com</t>
+  </si>
+  <si>
+    <t>9066712337</t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7C33C-1E6F-EF46-87FC-597C7CD0D47D}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1852,7 +1870,7 @@
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>141</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1892,7 +1910,7 @@
       <c r="E5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>148</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1932,7 +1950,7 @@
       <c r="E6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>153</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1972,7 +1990,7 @@
       <c r="E7" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>159</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1984,6 +2002,7 @@
       <c r="I7" s="2" t="s">
         <v>158</v>
       </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
@@ -2001,7 +2020,7 @@
       <c r="E8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>163</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -2013,180 +2032,225 @@
       <c r="I8" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2202,6 +2266,7 @@
     <hyperlink ref="F12" r:id="rId10" display="mailto:itachi123@gmail.com" xr:uid="{AB5771FA-B405-3D43-AD83-5031AEA235EB}"/>
     <hyperlink ref="F13" r:id="rId11" display="mailto:itachi123@gmail.com" xr:uid="{45C0D301-2445-8F41-A663-9E22C2937DAD}"/>
     <hyperlink ref="F14" r:id="rId12" display="mailto:itachi123@gmail.com" xr:uid="{7742987C-FA32-4D40-8DE2-0E0B85A57152}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{9B1F4A99-3C62-2C4A-8736-A801928839C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>